<commit_message>
Deploy website - based on 66e84562df404bac272dee3ab842ed8ac0b8c080
</commit_message>
<xml_diff>
--- a/secure/26P-Ainhoa.xlsx
+++ b/secure/26P-Ainhoa.xlsx
@@ -28,13 +28,13 @@
     <t>c</t>
   </si>
   <si>
-    <t>26P-Ainhoa-932461</t>
+    <t>26P-Ainhoa-689924</t>
   </si>
   <si>
-    <t>26P-Ainhoa-250098</t>
+    <t>26P-Ainhoa-1044564</t>
   </si>
   <si>
-    <t>26P-Ainhoa-683234</t>
+    <t>26P-Ainhoa-477074</t>
   </si>
 </sst>
 </file>
@@ -66,7 +66,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="F4f5f66b"/>
+        <fgColor rgb="Fd75d6b7"/>
       </patternFill>
     </fill>
   </fills>
@@ -427,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:TJ503"/>
+  <dimension ref="A1:VQ503"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1129,14 +1129,11 @@
       </c>
       <c r="M113" s="4"/>
     </row>
-    <row r="114" spans="1:530" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>-0.552</v>
       </c>
       <c r="M114" s="4"/>
-      <c r="TJ114" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
@@ -1324,11 +1321,14 @@
       </c>
       <c r="M145" s="4"/>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:452" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>-0.424</v>
       </c>
       <c r="M146" s="4"/>
+      <c r="QJ146" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
@@ -1474,14 +1474,11 @@
       </c>
       <c r="M170" s="4"/>
     </row>
-    <row r="171" spans="1:230" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>-0.324</v>
       </c>
       <c r="M171" s="4"/>
-      <c r="HV171" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
@@ -1873,11 +1870,14 @@
       </c>
       <c r="M236" s="4"/>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>-0.06</v>
       </c>
       <c r="M237" s="4"/>
+      <c r="BH237" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
@@ -3187,11 +3187,14 @@
       </c>
       <c r="M455" s="4"/>
     </row>
-    <row r="456" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:589" x14ac:dyDescent="0.25">
       <c r="A456" s="3">
         <v>0.816</v>
       </c>
       <c r="M456" s="4"/>
+      <c r="VQ456" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="457" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A457" s="3">
@@ -3367,14 +3370,11 @@
       </c>
       <c r="M485" s="4"/>
     </row>
-    <row r="486" spans="1:433" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A486" s="3">
         <v>0.936</v>
       </c>
       <c r="M486" s="4"/>
-      <c r="PQ486" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="487" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A487" s="3">

</xml_diff>